<commit_message>
Creacion metodo lagrange y newton interpolacion
</commit_message>
<xml_diff>
--- a/app/tables/tabla_secante.xlsx
+++ b/app/tables/tabla_secante.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,10 +460,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>-77</v>
+        <v>-75</v>
       </c>
       <c r="D2" t="n">
         <v>1.0005</v>
@@ -474,10 +474,10 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>-75</v>
+        <v>-71.6576262890778</v>
       </c>
       <c r="D3" t="n">
         <v>1.0005</v>
@@ -488,13 +488,13 @@
         <v>1</v>
       </c>
       <c r="B4" t="n">
-        <v>38.5</v>
+        <v>180.513140029589</v>
       </c>
       <c r="C4" t="n">
-        <v>-64.5981894738793</v>
+        <v>-44.059683603117</v>
       </c>
       <c r="D4" t="n">
-        <v>37.5</v>
+        <v>0.950142133705476</v>
       </c>
     </row>
     <row r="5">
@@ -502,13 +502,13 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>271.385621131759</v>
+        <v>454.331183985633</v>
       </c>
       <c r="C5" t="n">
-        <v>-34.0829006064861</v>
+        <v>-16.9007869850754</v>
       </c>
       <c r="D5" t="n">
-        <v>232.885621131759</v>
+        <v>0.602683798972299</v>
       </c>
     </row>
     <row r="6">
@@ -516,13 +516,13 @@
         <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>531.498429245955</v>
+        <v>624.726192982313</v>
       </c>
       <c r="C6" t="n">
-        <v>-10.3852733982163</v>
+        <v>-2.92090787921529</v>
       </c>
       <c r="D6" t="n">
-        <v>260.112808114196</v>
+        <v>0.272751504436287</v>
       </c>
     </row>
     <row r="7">
@@ -530,13 +530,13 @@
         <v>4</v>
       </c>
       <c r="B7" t="n">
-        <v>645.490543431168</v>
+        <v>660.327940364287</v>
       </c>
       <c r="C7" t="n">
-        <v>-1.31043625627018</v>
+        <v>-0.170222338927957</v>
       </c>
       <c r="D7" t="n">
-        <v>113.992114185213</v>
+        <v>0.0539152521129624</v>
       </c>
     </row>
     <row r="8">
@@ -544,13 +544,13 @@
         <v>5</v>
       </c>
       <c r="B8" t="n">
-        <v>661.95137870795</v>
+        <v>662.5311048556561</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0459865128422621</v>
+        <v>-0.0016467980762087</v>
       </c>
       <c r="D8" t="n">
-        <v>16.4608352767815</v>
+        <v>0.0033253751789487</v>
       </c>
     </row>
     <row r="9">
@@ -558,41 +558,13 @@
         <v>6</v>
       </c>
       <c r="B9" t="n">
-        <v>662.550039443012</v>
+        <v>662.552627355466</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.0001988252007549</v>
+        <v>-9.22459150842769e-07</v>
       </c>
       <c r="D9" t="n">
-        <v>0.598660735062481</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>7</v>
-      </c>
-      <c r="B10" t="n">
-        <v>662.5526390248421</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-3.00796045848983e-08</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0.0025995818300543</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>8</v>
-      </c>
-      <c r="B11" t="n">
-        <v>662.552639418184</v>
-      </c>
-      <c r="C11" t="n">
-        <v>-2.8421709430404e-14</v>
-      </c>
-      <c r="D11" t="n">
-        <v>3.9334156554105e-07</v>
+        <v>3.24842117008596e-05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>